<commit_message>
feat: :zap: Generating more artifacts and views to conclude the research.
</commit_message>
<xml_diff>
--- a/research-in-acc-sciences/accountant-profile-in-startups/kavanagh2008_top10_employers.xlsx
+++ b/research-in-acc-sciences/accountant-profile-in-startups/kavanagh2008_top10_employers.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>skill_en</t>
   </si>
@@ -90,12 +90,6 @@
   </si>
   <si>
     <t>Aprendizagem contínua / atualização / atualização de habilidades básicas</t>
-  </si>
-  <si>
-    <t>data_science</t>
-  </si>
-  <si>
-    <t>multiplas habilidades de TI</t>
   </si>
 </sst>
 </file>
@@ -425,9 +419,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -436,7 +432,7 @@
     <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -444,18 +440,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -463,7 +456,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -471,7 +464,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -479,7 +472,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -487,7 +480,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -495,7 +488,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -503,18 +496,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -522,7 +512,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>